<commit_message>
fixed incorrect combining of dictionaries when fetching existing meetings and webinars from zoom.
</commit_message>
<xml_diff>
--- a/InvitedTalks.xlsx
+++ b/InvitedTalks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lee/Sites/badgeserver.onsite/xltozoom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49FEC3C1-64F8-9843-A9E9-D0FEDC038A99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{668CCBAC-52B3-A84D-9ED3-A05ADAB7FBBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5160" windowWidth="40960" windowHeight="12000" xr2:uid="{24F3A499-F06E-3E44-802A-A6BEBE33E2A2}"/>
+    <workbookView xWindow="-20" yWindow="9760" windowWidth="40960" windowHeight="12000" xr2:uid="{24F3A499-F06E-3E44-802A-A6BEBE33E2A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -191,28 +191,28 @@
     <t>yoshua.umontreal@gmail.com, yann@fb.com</t>
   </si>
   <si>
-    <t>Timnit Gebru &lt;tgebru@gmail.com&gt;</t>
-  </si>
-  <si>
-    <t>Shakir Mohamed &lt;shakir.mohamed@gmail.com&gt;</t>
-  </si>
-  <si>
-    <t>Kyunghyun Cho &lt;kyunghyun.cho@nyu.edu&gt;</t>
-  </si>
-  <si>
-    <t>Asja Fischer &lt;asja.fischer@rub.de&gt;</t>
-  </si>
-  <si>
-    <t>Martha White &lt;whitem@ualberta.ca&gt;</t>
-  </si>
-  <si>
-    <t>Gabriel Synnaeve &lt;gab@fb.com&gt;</t>
-  </si>
-  <si>
-    <t>Dawn Song &lt;dawnsong@gmail.com&gt;</t>
-  </si>
-  <si>
-    <t>Alexander Rush &lt;sasha.rush@gmail.com&gt;</t>
+    <t>Timnit Gebru &lt;tgebru+iclrzoom@gmail.com&gt;</t>
+  </si>
+  <si>
+    <t>Shakir Mohamed &lt;shakir.mohamed+iclrzoom@gmail.com&gt;</t>
+  </si>
+  <si>
+    <t>Kyunghyun Cho &lt;kyunghyun.cho+iclrzoom@nyu.edu&gt;</t>
+  </si>
+  <si>
+    <t>Asja Fischer &lt;asja.fischer+iclrzoom@gmail.com&gt;</t>
+  </si>
+  <si>
+    <t>Martha White &lt;whitem+iclrzoom@ualberta.ca&gt;</t>
+  </si>
+  <si>
+    <t>Gabriel Synnaeve &lt;gabriel.synnaeve+iclrzoom@gmail.com&gt;</t>
+  </si>
+  <si>
+    <t>Dawn Song &lt;dawnsong+iclrzoom@gmail.com&gt;</t>
+  </si>
+  <si>
+    <t>Alexander Rush &lt;sasha.rush+iclrzoom@gmail.com&gt;</t>
   </si>
 </sst>
 </file>
@@ -581,7 +581,7 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -594,7 +594,7 @@
     <col min="6" max="6" width="12.33203125" customWidth="1"/>
     <col min="8" max="8" width="33.6640625" customWidth="1"/>
     <col min="9" max="9" width="32.33203125" customWidth="1"/>
-    <col min="10" max="10" width="37" customWidth="1"/>
+    <col min="10" max="10" width="51.6640625" customWidth="1"/>
     <col min="11" max="11" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
adding function to create chair accounts
</commit_message>
<xml_diff>
--- a/InvitedTalks.xlsx
+++ b/InvitedTalks.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lee/Sites/badgeserver.onsite/xltozoom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{668CCBAC-52B3-A84D-9ED3-A05ADAB7FBBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414A03DF-9054-0E41-8839-4CFDF1FFD945}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="9760" windowWidth="40960" windowHeight="12000" xr2:uid="{24F3A499-F06E-3E44-802A-A6BEBE33E2A2}"/>
+    <workbookView xWindow="0" yWindow="9760" windowWidth="46260" windowHeight="12320" xr2:uid="{24F3A499-F06E-3E44-802A-A6BEBE33E2A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="zoom user ids" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="61">
   <si>
     <t>timezone</t>
   </si>
@@ -179,9 +180,6 @@
     <t>iclrconf+Jordan@gmail.com</t>
   </si>
   <si>
-    <t>zoom_user_id</t>
-  </si>
-  <si>
     <t>panelists</t>
   </si>
   <si>
@@ -203,9 +201,6 @@
     <t>Asja Fischer &lt;asja.fischer+iclrzoom@gmail.com&gt;</t>
   </si>
   <si>
-    <t>Martha White &lt;whitem+iclrzoom@ualberta.ca&gt;</t>
-  </si>
-  <si>
     <t>Gabriel Synnaeve &lt;gabriel.synnaeve+iclrzoom@gmail.com&gt;</t>
   </si>
   <si>
@@ -213,6 +208,15 @@
   </si>
   <si>
     <t>Alexander Rush &lt;sasha.rush+iclrzoom@gmail.com&gt;</t>
+  </si>
+  <si>
+    <t>Martha White &lt;iclrconf+mwhite@gmail.com&gt;</t>
+  </si>
+  <si>
+    <t>host_zoom_user_email</t>
+  </si>
+  <si>
+    <t>leetncamp+iclr@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -581,7 +585,7 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="K2" sqref="K2:K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -624,13 +628,13 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>8</v>
@@ -668,10 +672,10 @@
         <v>33</v>
       </c>
       <c r="J2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K2" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -700,10 +704,10 @@
         <v>32</v>
       </c>
       <c r="J3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K3" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -732,10 +736,10 @@
         <v>29</v>
       </c>
       <c r="J4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K4" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -764,10 +768,10 @@
         <v>27</v>
       </c>
       <c r="J5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K5" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -796,10 +800,10 @@
         <v>24</v>
       </c>
       <c r="J6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="K6" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -828,10 +832,10 @@
         <v>22</v>
       </c>
       <c r="J7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K7" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -857,13 +861,13 @@
         <v>19</v>
       </c>
       <c r="I8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K8" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -892,10 +896,10 @@
         <v>18</v>
       </c>
       <c r="J9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K9" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -905,4 +909,59 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EEAF067-0895-594C-9B35-2F2C3DE8EFE9}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>